<commit_message>
added a new estimate
</commit_message>
<xml_diff>
--- a/data/av_estimates_dummytest.xlsx
+++ b/data/av_estimates_dummytest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e72fa63d99f79ef2/Documents/Uni Agrarwissenschaften/Master/10. Semester/Decision Analysis/DecisionAnalysis_Agrivoltaics2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{71A86003-2426-4F5E-BBFF-DA1EB23C67AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{71A86003-2426-4F5E-BBFF-DA1EB23C67AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75415C39-BC08-4732-B826-CE95FE1408C8}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4A43B7D9-233E-410A-8DA4-F1298413F588}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="38">
   <si>
     <t>variable</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>agrovoltaics_int_no_involvement_by_population</t>
   </si>
 </sst>
 </file>
@@ -497,15 +500,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0747F3B3-4129-44D5-B3F6-271B8C0ECC7B}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="45.42578125" customWidth="1"/>
     <col min="6" max="6" width="26" customWidth="1"/>
   </cols>
   <sheetData>
@@ -831,6 +834,11 @@
         <v>36</v>
       </c>
     </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New estimates, partially dummy
</commit_message>
<xml_diff>
--- a/data/av_estimates_dummytest.xlsx
+++ b/data/av_estimates_dummytest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e72fa63d99f79ef2/Documents/Uni Agrarwissenschaften/Master/10. Semester/Decision Analysis/DecisionAnalysis_Agrivoltaics2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{71A86003-2426-4F5E-BBFF-DA1EB23C67AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75415C39-BC08-4732-B826-CE95FE1408C8}"/>
+  <xr:revisionPtr revIDLastSave="36" documentId="8_{71A86003-2426-4F5E-BBFF-DA1EB23C67AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77539D55-864C-4A74-AE30-D79C8751ACC4}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4A43B7D9-233E-410A-8DA4-F1298413F588}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="25">
   <si>
     <t>variable</t>
   </si>
@@ -64,91 +64,52 @@
     <t>posnorm</t>
   </si>
   <si>
-    <t>ha</t>
-  </si>
-  <si>
-    <t>Farm area in ha</t>
-  </si>
-  <si>
-    <t>yield_per_ha</t>
-  </si>
-  <si>
-    <t>Yield/ha</t>
-  </si>
-  <si>
-    <t>loss_after_harvest</t>
-  </si>
-  <si>
-    <t>market_price</t>
-  </si>
-  <si>
-    <t>demand</t>
-  </si>
-  <si>
-    <t>workload</t>
-  </si>
-  <si>
-    <t>price_work</t>
-  </si>
-  <si>
-    <t>energy_irrigation</t>
-  </si>
-  <si>
-    <t>energy_management</t>
-  </si>
-  <si>
-    <t>price_energy_kwh</t>
-  </si>
-  <si>
-    <t>water_consumption</t>
-  </si>
-  <si>
-    <t>price_water_L</t>
-  </si>
-  <si>
-    <t>pest_control</t>
-  </si>
-  <si>
-    <t>Yield / ha</t>
-  </si>
-  <si>
-    <t>Loss after harvest / ha</t>
-  </si>
-  <si>
-    <t>Market price as multiplicator</t>
-  </si>
-  <si>
-    <t>Price work as multiplicator</t>
-  </si>
-  <si>
-    <t>Energy management as multiplicator</t>
-  </si>
-  <si>
-    <t>Pest control as multiplicator</t>
-  </si>
-  <si>
-    <t>Workload / ha</t>
-  </si>
-  <si>
-    <t>Demand as multiplicator</t>
-  </si>
-  <si>
-    <t>Energy irrigation / ha</t>
-  </si>
-  <si>
-    <t>Price water / L</t>
-  </si>
-  <si>
-    <t>Water consumption L/ ha</t>
-  </si>
-  <si>
-    <t>Price energy  kwh/ha</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>agrovoltaics_int_no_involvement_by_population</t>
+    <t>av_int_no_involvement_by_population</t>
+  </si>
+  <si>
+    <t>av_int_event_photovoltaic_panels</t>
+  </si>
+  <si>
+    <t>av_crop_ha</t>
+  </si>
+  <si>
+    <t>av_crop_yield_t_ha</t>
+  </si>
+  <si>
+    <t>av_crop_profit_EUR_t</t>
+  </si>
+  <si>
+    <t>av_energy_ha</t>
+  </si>
+  <si>
+    <t>av_energy_yield_kwh_ha</t>
+  </si>
+  <si>
+    <t>av_energy_profit_EUR_kwh</t>
+  </si>
+  <si>
+    <t>av_int_cost_search_panels</t>
+  </si>
+  <si>
+    <t>av_int_cost_search_location</t>
+  </si>
+  <si>
+    <t>av_int_cost_photovoltaic_panels</t>
+  </si>
+  <si>
+    <t>av_int_cost_ground_preparation</t>
+  </si>
+  <si>
+    <t>av_int_cost_installation</t>
+  </si>
+  <si>
+    <t>av_int_cost_training</t>
+  </si>
+  <si>
+    <t>av_int_cost_reparation</t>
+  </si>
+  <si>
+    <t>av_int_benefit_shade</t>
   </si>
 </sst>
 </file>
@@ -500,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0747F3B3-4129-44D5-B3F6-271B8C0ECC7B}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,7 +501,7 @@
         <v>9</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -552,7 +513,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" t="s">
         <v>9</v>
@@ -560,214 +521,214 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
       <c r="D3">
-        <v>600</v>
+        <v>1</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="G6" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
       </c>
       <c r="D7">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
       </c>
       <c r="D8">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
       <c r="D9">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10">
-        <v>0.85</v>
+        <v>0</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
       </c>
       <c r="D10">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C11" t="s">
         <v>7</v>
       </c>
       <c r="D11">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="G11" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -776,67 +737,131 @@
         <v>7</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="G12" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
       </c>
       <c r="D14">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
       </c>
       <c r="F14" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="G14" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>